<commit_message>
perbaikan migration travel dan upload template excel travel admin kanwil
</commit_message>
<xml_diff>
--- a/public/template/format_travel.xlsx
+++ b/public/template/format_travel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rival\Documents\code\haji\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EA92855-59F5-40EB-8B56-38DBA7D9F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EBAE43-445C-4495-B36B-BD0D2A43F9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A01BAFE1-9659-4408-B97E-069FFF078BA6}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{A01BAFE1-9659-4408-B97E-069FFF078BA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>No.</t>
-  </si>
-  <si>
     <t>Penyelenggara</t>
   </si>
   <si>
@@ -57,22 +54,25 @@
     <t>Tanggal</t>
   </si>
   <si>
-    <t>Jml Akre</t>
-  </si>
-  <si>
-    <t>tanggal akreditasi</t>
-  </si>
-  <si>
-    <t>lembaga akreditasi</t>
-  </si>
-  <si>
     <t>Telepon</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Kab/Kota</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Jml_Akreditasi</t>
+  </si>
+  <si>
+    <t>tanggal_akreditasi</t>
+  </si>
+  <si>
+    <t>lembaga_akreditasi</t>
+  </si>
+  <si>
+    <t>kab_kota</t>
   </si>
 </sst>
 </file>
@@ -440,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7682ADC2-DFA5-4AAC-9C50-DBD151447664}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,40 +453,40 @@
   <sheetData>
     <row r="1" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>12</v>
@@ -504,5 +504,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>